<commit_message>
Update instructor names in horarios/1-2024.json
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024.xlsx
+++ b/static/horarios/1-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C0980-3A2B-4589-B744-3638EF8B8338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EF3B4B-6131-4679-867B-2518E5CA4697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024.xlsxPROPUESTAS_ÁREA_I_2024" hidden="1">PROPUESTAS_ÁREA_I_2024[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024.xlsxPROPUESTAS_ÁREA_I_20241" hidden="1">PROPUESTAS_ÁREA_I_2024[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">CONSOLIDADO_I_2024!$A$2:$DA$396</definedName>
     <definedName name="SegmentaciónDeDatos_14_15L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_20_21L">#N/A</definedName>
@@ -102,7 +102,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROPUESTAS_ÁREA_I_2024" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024.xlsxPROPUESTAS_ÁREA_I_2024"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024.xlsxPROPUESTAS_ÁREA_I_20241"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="545">
   <si>
     <t>Source.Name</t>
   </si>
@@ -1743,6 +1743,9 @@
   </si>
   <si>
     <t>ASTRID YULIETH GUZMÁN BURBANO</t>
+  </si>
+  <si>
+    <t>NUEVO ACTIVIDAD FISICA</t>
   </si>
 </sst>
 </file>
@@ -2751,11 +2754,6 @@
       <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
@@ -6606,7 +6604,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -6628,8 +6626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754D4503-1E10-47C8-980C-181088D300A7}">
   <dimension ref="A1:DI397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N143" sqref="N143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8759,7 +8757,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>278</v>
+        <v>544</v>
       </c>
       <c r="P35">
         <v>2</v>
@@ -13314,7 +13312,7 @@
         <v>1</v>
       </c>
       <c r="N115" t="s">
-        <v>278</v>
+        <v>544</v>
       </c>
       <c r="P115">
         <v>2</v>
@@ -14969,7 +14967,7 @@
         <v>1</v>
       </c>
       <c r="N143" t="s">
-        <v>278</v>
+        <v>544</v>
       </c>
       <c r="P143">
         <v>2</v>
@@ -17221,7 +17219,7 @@
         <v>1</v>
       </c>
       <c r="N186" t="s">
-        <v>278</v>
+        <v>544</v>
       </c>
       <c r="P186">
         <v>2</v>
@@ -27468,7 +27466,7 @@
         <v>1</v>
       </c>
       <c r="N394" t="s">
-        <v>278</v>
+        <v>544</v>
       </c>
       <c r="P394">
         <v>2</v>

</xml_diff>

<commit_message>
Strip leading and trailing whitespace from the 'ficha' form input
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024.xlsx
+++ b/static/horarios/1-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C9039-774D-4D37-BFAC-3E88C665709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42462341-8721-4C0E-96FF-A5768740C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$377</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -104,7 +104,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="503">
   <si>
     <t>Source.Name</t>
   </si>
@@ -1324,9 +1324,6 @@
     <t>GESTIONAR PROCESOS PROPIOS DE LA CULTURA EMPRENDEDORAY EMPRESARIA DE ACUERDO CON EL PERFIL PERSONAL Y LOS REQUERIMIENTOS DE LOS CONTEXTOS PRODICTIVO Y SOCIAL - Emprendimiento</t>
   </si>
   <si>
-    <t>2875572 A</t>
-  </si>
-  <si>
     <t>TEC. ELABORACIÓN AUDIOVISUALES</t>
   </si>
   <si>
@@ -1588,6 +1585,15 @@
     <t>2875444 A</t>
   </si>
   <si>
+    <t>2742580 C</t>
+  </si>
+  <si>
+    <t>TEC303</t>
+  </si>
+  <si>
+    <t>2875586 A</t>
+  </si>
+  <si>
     <t>6-7S</t>
   </si>
   <si>
@@ -1616,9 +1622,6 @@
   </si>
   <si>
     <t>21-22S</t>
-  </si>
-  <si>
-    <t>2742580 C</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1704,6 +1707,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2571,11 +2575,6 @@
       <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
@@ -4987,231 +4986,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D30:E47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="16">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="17">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Recuento distinto de FICHA" fld="1" subtotal="count" baseField="0" baseItem="0">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FABC7310-3BB5-11E1-824E-6D434824019B}">
-          <x15:dataField isCountDistinct="1"/>
-        </ext>
-      </extLst>
-    </dataField>
-  </dataFields>
-  <pivotHierarchies count="109">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Recuento distinto de FICHA"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="2"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
-        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E51D2C13-18A8-44E4-9514-17D00C659F63}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B82" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
@@ -5661,6 +5435,231 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
     <rowHierarchyUsage hierarchyUsage="13"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
+        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D30:E47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="16">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Recuento distinto de FICHA" fld="1" subtotal="count" baseField="0" baseItem="0">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FABC7310-3BB5-11E1-824E-6D434824019B}">
+          <x15:dataField isCountDistinct="1"/>
+        </ext>
+      </extLst>
+    </dataField>
+  </dataFields>
+  <pivotHierarchies count="109">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Recuento distinto de FICHA"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="2"/>
   </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -6108,7 +6107,7 @@
     <tableColumn id="97" xr3:uid="{C47FF5A8-51B9-41AF-8D63-CEB7C92ACB49}" uniqueName="97" name="21-22V" totalsRowFunction="custom" queryTableFieldId="97">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[21-22V])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DD845AE9-38B6-4A80-8432-09E4AAC72E7D}" uniqueName="1" name="6-7S" queryTableFieldId="105"/>
+    <tableColumn id="1" xr3:uid="{DA68D4F0-B1F1-4D08-8BBA-5EE8F6703898}" uniqueName="1" name="6-7S" queryTableFieldId="105"/>
     <tableColumn id="98" xr3:uid="{25044A8C-0253-4E22-980E-977A3B5C6C59}" uniqueName="98" name="7-8S" totalsRowFunction="custom" queryTableFieldId="98">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[7-8S])</totalsRowFormula>
     </tableColumn>
@@ -6130,14 +6129,14 @@
     <tableColumn id="104" xr3:uid="{FD79054B-1F48-4B17-8E3F-E8071CD3F12B}" uniqueName="104" name="13-14S" totalsRowFunction="custom" queryTableFieldId="104">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[13-14S])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="106" xr3:uid="{F040B160-123F-41F3-833E-B05E986C4DBF}" uniqueName="106" name="14-15S" queryTableFieldId="106"/>
-    <tableColumn id="107" xr3:uid="{10D02C96-E34A-4B40-8233-841B3C266A70}" uniqueName="107" name="15-16S" queryTableFieldId="107"/>
-    <tableColumn id="108" xr3:uid="{D5E03B02-FE6E-48D4-A664-5FAA42BACB7D}" uniqueName="108" name="16-17S" queryTableFieldId="108"/>
-    <tableColumn id="109" xr3:uid="{758A1885-478F-4515-9C8C-DF421652753D}" uniqueName="109" name="17-18S" queryTableFieldId="109"/>
-    <tableColumn id="110" xr3:uid="{9CCED529-3CAC-460F-AD3A-DD847BD4918E}" uniqueName="110" name="18-19S" queryTableFieldId="110"/>
-    <tableColumn id="111" xr3:uid="{ED6351E4-53CD-42B7-8B6E-E94C6269E09D}" uniqueName="111" name="19-20S" queryTableFieldId="111"/>
-    <tableColumn id="112" xr3:uid="{018626A8-6BC4-4D1A-AF55-EB05137C4C4C}" uniqueName="112" name="20-21S" queryTableFieldId="112"/>
-    <tableColumn id="113" xr3:uid="{DA218E77-EC56-4B52-B643-4E7D054D4396}" uniqueName="113" name="21-22S" queryTableFieldId="113"/>
+    <tableColumn id="106" xr3:uid="{F7C9ADE6-EB7A-429A-8C5A-DB58B52CA8BD}" uniqueName="106" name="14-15S" queryTableFieldId="106"/>
+    <tableColumn id="107" xr3:uid="{C0F52894-9EE5-45F0-8371-0D086A3E656E}" uniqueName="107" name="15-16S" queryTableFieldId="107"/>
+    <tableColumn id="108" xr3:uid="{241E9FC5-1B0A-43B4-842D-347B3CB21248}" uniqueName="108" name="16-17S" queryTableFieldId="108"/>
+    <tableColumn id="109" xr3:uid="{DB43EF92-8B09-47AF-AEC7-A29A0EF9AAC6}" uniqueName="109" name="17-18S" queryTableFieldId="109"/>
+    <tableColumn id="110" xr3:uid="{1DD59851-2B16-49E1-9997-DE25D84F36D4}" uniqueName="110" name="18-19S" queryTableFieldId="110"/>
+    <tableColumn id="111" xr3:uid="{9921D150-7286-485E-A9EE-60E5572AC3E4}" uniqueName="111" name="19-20S" queryTableFieldId="111"/>
+    <tableColumn id="112" xr3:uid="{8D7D2FF1-C4A3-4428-8658-87BE8379F37F}" uniqueName="112" name="20-21S" queryTableFieldId="112"/>
+    <tableColumn id="113" xr3:uid="{4E35FCDC-686A-4555-AD55-FB43AD30547C}" uniqueName="113" name="21-22S" queryTableFieldId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6413,10 +6412,10 @@
 </file>
 
 <file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{3C9AC298-184D-4F56-A345-DA071939C279}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{160A34EE-E4AE-446D-B0BE-F0187B8A3549}">
   <we:reference id="wa104380263" version="1.1.3.0" store="es-ES" storeType="OMEX"/>
   <we:alternateReferences>
-    <we:reference id="WA104380263" version="1.1.3.0" store="WA104380263" storeType="OMEX"/>
+    <we:reference id="wa104380263" version="1.1.3.0" store="WA104380263" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties/>
   <we:bindings/>
@@ -6428,8 +6427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C46E5B-3CE7-4F67-9F7E-3BDF34AAB992}">
   <dimension ref="A1:DI378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView tabSelected="1" topLeftCell="CJ353" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:DI377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6470,10 +6469,10 @@
     <row r="1" spans="1:113" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P1" s="1">
         <f>SUBTOTAL(9,PROGRAMACIONES_PARCIALES[HORAS SEMANAL])</f>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
@@ -6491,7 +6490,7 @@
       <c r="AF1" s="6"/>
       <c r="AG1" s="6"/>
       <c r="AH1" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="6"/>
@@ -6509,7 +6508,7 @@
       <c r="AV1" s="6"/>
       <c r="AW1" s="6"/>
       <c r="AX1" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AY1" s="6"/>
       <c r="AZ1" s="6"/>
@@ -6527,7 +6526,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
       <c r="BN1" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="BO1" s="6"/>
       <c r="BP1" s="6"/>
@@ -6545,7 +6544,7 @@
       <c r="CB1" s="6"/>
       <c r="CC1" s="6"/>
       <c r="CD1" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="CE1" s="6"/>
       <c r="CF1" s="6"/>
@@ -6564,7 +6563,7 @@
       <c r="CS1" s="6"/>
       <c r="CT1" s="5"/>
       <c r="CU1" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="CV1" s="6"/>
       <c r="CW1" s="6"/>
@@ -6865,53 +6864,53 @@
       <c r="CS2" t="s">
         <v>96</v>
       </c>
-      <c r="CT2" t="s">
-        <v>491</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>492</v>
-      </c>
-      <c r="CV2" t="s">
+      <c r="CT2" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="CU2" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="CV2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CW2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="CX2" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="CY2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="CZ2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DA2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="DB2" t="s">
-        <v>493</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>494</v>
-      </c>
-      <c r="DD2" t="s">
+      <c r="DB2" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DC2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="DF2" t="s">
+      <c r="DD2" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="DG2" t="s">
+      <c r="DE2" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="DH2" t="s">
+      <c r="DF2" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="DI2" t="s">
+      <c r="DG2" s="7" t="s">
         <v>500</v>
+      </c>
+      <c r="DH2" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="DI2" s="7" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:113" x14ac:dyDescent="0.3">
@@ -7517,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -7718,7 +7717,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P14">
         <v>2</v>
@@ -7969,7 +7968,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P18">
         <v>2</v>
@@ -8146,7 +8145,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P21">
         <v>2</v>
@@ -8246,7 +8245,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P23">
         <v>2</v>
@@ -8337,7 +8336,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P25">
         <v>2</v>
@@ -8918,7 +8917,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P35">
         <v>2</v>
@@ -9011,65 +9010,65 @@
       <c r="Q37">
         <v>240</v>
       </c>
-      <c r="Z37">
-        <v>4</v>
-      </c>
-      <c r="AA37">
-        <v>4</v>
-      </c>
-      <c r="AB37">
-        <v>4</v>
-      </c>
-      <c r="AC37">
-        <v>4</v>
-      </c>
-      <c r="AP37">
-        <v>4</v>
-      </c>
-      <c r="AQ37">
-        <v>4</v>
-      </c>
-      <c r="AR37">
-        <v>4</v>
-      </c>
-      <c r="AS37">
-        <v>4</v>
-      </c>
-      <c r="BD37">
-        <v>4</v>
-      </c>
-      <c r="BE37">
-        <v>4</v>
-      </c>
-      <c r="BF37">
-        <v>4</v>
-      </c>
-      <c r="BG37">
-        <v>4</v>
-      </c>
-      <c r="BV37">
-        <v>4</v>
-      </c>
-      <c r="BW37">
-        <v>4</v>
-      </c>
-      <c r="BX37">
-        <v>4</v>
-      </c>
-      <c r="BY37">
-        <v>4</v>
-      </c>
-      <c r="CL37">
-        <v>4</v>
-      </c>
-      <c r="CM37">
-        <v>4</v>
-      </c>
-      <c r="CN37">
-        <v>4</v>
-      </c>
-      <c r="CO37">
-        <v>4</v>
+      <c r="Z37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AP37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BD37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BE37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BF37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BG37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BV37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BW37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BX37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BY37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CL37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CM37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CN37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CO37" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:105" x14ac:dyDescent="0.3">
@@ -9115,11 +9114,11 @@
       <c r="Q38">
         <v>24</v>
       </c>
-      <c r="X38">
-        <v>4</v>
-      </c>
-      <c r="Y38">
-        <v>4</v>
+      <c r="X38" t="s">
+        <v>491</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:105" x14ac:dyDescent="0.3">
@@ -9165,11 +9164,11 @@
       <c r="Q39">
         <v>24</v>
       </c>
-      <c r="AN39">
-        <v>4</v>
-      </c>
-      <c r="AO39">
-        <v>4</v>
+      <c r="AN39" t="s">
+        <v>491</v>
+      </c>
+      <c r="AO39" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:105" x14ac:dyDescent="0.3">
@@ -9215,11 +9214,11 @@
       <c r="Q40">
         <v>24</v>
       </c>
-      <c r="BH40">
-        <v>4</v>
-      </c>
-      <c r="BI40">
-        <v>4</v>
+      <c r="BH40" t="s">
+        <v>491</v>
+      </c>
+      <c r="BI40" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:105" x14ac:dyDescent="0.3">
@@ -9265,11 +9264,11 @@
       <c r="Q41">
         <v>24</v>
       </c>
-      <c r="CJ41">
-        <v>4</v>
-      </c>
-      <c r="CK41">
-        <v>4</v>
+      <c r="CJ41" t="s">
+        <v>491</v>
+      </c>
+      <c r="CK41" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:105" x14ac:dyDescent="0.3">
@@ -9306,11 +9305,11 @@
       <c r="Q42">
         <v>24</v>
       </c>
-      <c r="BT42">
-        <v>4</v>
-      </c>
-      <c r="BU42">
-        <v>4</v>
+      <c r="BT42" t="s">
+        <v>491</v>
+      </c>
+      <c r="BU42" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:105" x14ac:dyDescent="0.3">
@@ -9932,7 +9931,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P53">
         <v>2</v>
@@ -10098,7 +10097,7 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P55">
         <v>2</v>
@@ -10422,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P61">
         <v>2</v>
@@ -10743,7 +10742,7 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P67">
         <v>2</v>
@@ -10793,7 +10792,7 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P68">
         <v>2</v>
@@ -10936,77 +10935,77 @@
       <c r="Q71">
         <v>288</v>
       </c>
-      <c r="R71">
-        <v>4</v>
-      </c>
-      <c r="S71">
-        <v>4</v>
-      </c>
-      <c r="T71">
-        <v>4</v>
-      </c>
-      <c r="U71">
-        <v>4</v>
-      </c>
-      <c r="AH71">
-        <v>4</v>
-      </c>
-      <c r="AI71">
-        <v>4</v>
-      </c>
-      <c r="AJ71">
-        <v>4</v>
-      </c>
-      <c r="AK71">
-        <v>4</v>
-      </c>
-      <c r="AL71">
-        <v>4</v>
-      </c>
-      <c r="AM71">
-        <v>4</v>
-      </c>
-      <c r="AX71">
-        <v>4</v>
-      </c>
-      <c r="AY71">
-        <v>4</v>
-      </c>
-      <c r="AZ71">
-        <v>4</v>
-      </c>
-      <c r="BA71">
-        <v>4</v>
-      </c>
-      <c r="BB71">
-        <v>4</v>
-      </c>
-      <c r="BC71">
-        <v>4</v>
-      </c>
-      <c r="BN71">
-        <v>4</v>
-      </c>
-      <c r="BO71">
-        <v>4</v>
-      </c>
-      <c r="BP71">
-        <v>4</v>
-      </c>
-      <c r="BQ71">
-        <v>4</v>
-      </c>
-      <c r="CD71">
-        <v>4</v>
-      </c>
-      <c r="CE71">
-        <v>4</v>
-      </c>
-      <c r="CF71">
-        <v>4</v>
-      </c>
-      <c r="CG71">
-        <v>4</v>
+      <c r="R71" t="s">
+        <v>491</v>
+      </c>
+      <c r="S71" t="s">
+        <v>491</v>
+      </c>
+      <c r="T71" t="s">
+        <v>491</v>
+      </c>
+      <c r="U71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AI71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AJ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AK71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AL71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AX71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AY71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AZ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BA71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BC71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BN71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BO71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BP71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BQ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CD71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CE71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CF71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CG71" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="72" spans="1:105" x14ac:dyDescent="0.3">
@@ -11052,11 +11051,11 @@
       <c r="Q72">
         <v>24</v>
       </c>
-      <c r="BR72">
-        <v>4</v>
-      </c>
-      <c r="BS72">
-        <v>4</v>
+      <c r="BR72" t="s">
+        <v>491</v>
+      </c>
+      <c r="BS72" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="73" spans="1:105" x14ac:dyDescent="0.3">
@@ -11102,11 +11101,11 @@
       <c r="Q73">
         <v>24</v>
       </c>
-      <c r="CH73">
-        <v>4</v>
-      </c>
-      <c r="CI73">
-        <v>4</v>
+      <c r="CH73" t="s">
+        <v>491</v>
+      </c>
+      <c r="CI73" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="74" spans="1:105" x14ac:dyDescent="0.3">
@@ -11143,11 +11142,11 @@
       <c r="Q74">
         <v>24</v>
       </c>
-      <c r="V74">
-        <v>4</v>
-      </c>
-      <c r="W74">
-        <v>4</v>
+      <c r="V74" t="s">
+        <v>491</v>
+      </c>
+      <c r="W74" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="75" spans="1:105" x14ac:dyDescent="0.3">
@@ -11456,7 +11455,7 @@
         <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C80" t="s">
         <v>105</v>
@@ -11500,7 +11499,7 @@
         <v>103</v>
       </c>
       <c r="B81" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C81" t="s">
         <v>105</v>
@@ -11622,7 +11621,7 @@
         <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C82" t="s">
         <v>105</v>
@@ -11663,7 +11662,7 @@
         <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C83" t="s">
         <v>105</v>
@@ -11713,7 +11712,7 @@
         <v>103</v>
       </c>
       <c r="B84" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C84" t="s">
         <v>105</v>
@@ -11745,7 +11744,7 @@
         <v>103</v>
       </c>
       <c r="B85" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C85" t="s">
         <v>105</v>
@@ -11867,7 +11866,7 @@
         <v>103</v>
       </c>
       <c r="B86" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C86" t="s">
         <v>105</v>
@@ -11917,7 +11916,7 @@
         <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C87" t="s">
         <v>105</v>
@@ -11938,7 +11937,7 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P87">
         <v>2</v>
@@ -12851,7 +12850,7 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O104" t="s">
         <v>195</v>
@@ -13502,7 +13501,7 @@
         <v>1</v>
       </c>
       <c r="N116" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O116" t="s">
         <v>215</v>
@@ -15568,7 +15567,7 @@
         <v>1</v>
       </c>
       <c r="N153" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O153" t="s">
         <v>195</v>
@@ -16164,7 +16163,7 @@
         <v>1</v>
       </c>
       <c r="N163" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O163" t="s">
         <v>195</v>
@@ -16365,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O166" t="s">
         <v>255</v>
@@ -17119,7 +17118,7 @@
         <v>184</v>
       </c>
       <c r="B180" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C180" t="s">
         <v>186</v>
@@ -17175,7 +17174,7 @@
         <v>184</v>
       </c>
       <c r="B181" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C181" t="s">
         <v>186</v>
@@ -17228,7 +17227,7 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C182" t="s">
         <v>186</v>
@@ -17305,7 +17304,7 @@
         <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C183" t="s">
         <v>186</v>
@@ -17358,7 +17357,7 @@
         <v>184</v>
       </c>
       <c r="B184" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C184" t="s">
         <v>186</v>
@@ -17411,7 +17410,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C185" t="s">
         <v>186</v>
@@ -17715,7 +17714,7 @@
         <v>1</v>
       </c>
       <c r="N190" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O190" t="s">
         <v>215</v>
@@ -18036,7 +18035,7 @@
         <v>1</v>
       </c>
       <c r="N196" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O196" t="s">
         <v>195</v>
@@ -18410,7 +18409,7 @@
         <v>1</v>
       </c>
       <c r="N203" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O203" t="s">
         <v>195</v>
@@ -19099,7 +19098,7 @@
         <v>1</v>
       </c>
       <c r="N216" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O216" t="s">
         <v>195</v>
@@ -20585,7 +20584,7 @@
         <v>1</v>
       </c>
       <c r="N242" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P242">
         <v>2</v>
@@ -20685,7 +20684,7 @@
         <v>1</v>
       </c>
       <c r="N244" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P244">
         <v>2</v>
@@ -22657,7 +22656,7 @@
         <v>1</v>
       </c>
       <c r="N282" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P282">
         <v>2</v>
@@ -22707,7 +22706,7 @@
         <v>1</v>
       </c>
       <c r="N283" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P283">
         <v>2</v>
@@ -22917,7 +22916,7 @@
         <v>1</v>
       </c>
       <c r="N286" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P286">
         <v>2</v>
@@ -24095,7 +24094,7 @@
         <v>1</v>
       </c>
       <c r="N305" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P305">
         <v>2</v>
@@ -24685,13 +24684,13 @@
         <v>361</v>
       </c>
       <c r="B315" t="s">
+        <v>492</v>
+      </c>
+      <c r="C315" t="s">
         <v>403</v>
       </c>
-      <c r="C315" t="s">
+      <c r="D315" t="s">
         <v>404</v>
-      </c>
-      <c r="D315" t="s">
-        <v>405</v>
       </c>
       <c r="E315">
         <v>1</v>
@@ -24700,7 +24699,7 @@
         <v>216</v>
       </c>
       <c r="G315" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H315">
         <v>1</v>
@@ -24712,7 +24711,7 @@
         <v>1</v>
       </c>
       <c r="N315" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P315">
         <v>4</v>
@@ -24738,13 +24737,13 @@
         <v>361</v>
       </c>
       <c r="B316" t="s">
+        <v>492</v>
+      </c>
+      <c r="C316" t="s">
         <v>403</v>
       </c>
-      <c r="C316" t="s">
+      <c r="D316" t="s">
         <v>404</v>
-      </c>
-      <c r="D316" t="s">
-        <v>405</v>
       </c>
       <c r="E316">
         <v>1</v>
@@ -24753,7 +24752,7 @@
         <v>262</v>
       </c>
       <c r="G316" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H316">
         <v>1</v>
@@ -24768,7 +24767,7 @@
         <v>1</v>
       </c>
       <c r="N316" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P316">
         <v>20</v>
@@ -24842,13 +24841,13 @@
         <v>361</v>
       </c>
       <c r="B317" t="s">
+        <v>492</v>
+      </c>
+      <c r="C317" t="s">
         <v>403</v>
       </c>
-      <c r="C317" t="s">
+      <c r="D317" t="s">
         <v>404</v>
-      </c>
-      <c r="D317" t="s">
-        <v>405</v>
       </c>
       <c r="E317">
         <v>1</v>
@@ -24892,13 +24891,13 @@
         <v>361</v>
       </c>
       <c r="B318" t="s">
+        <v>492</v>
+      </c>
+      <c r="C318" t="s">
         <v>403</v>
       </c>
-      <c r="C318" t="s">
+      <c r="D318" t="s">
         <v>404</v>
-      </c>
-      <c r="D318" t="s">
-        <v>405</v>
       </c>
       <c r="E318">
         <v>1</v>
@@ -24922,7 +24921,7 @@
         <v>1</v>
       </c>
       <c r="N318" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P318">
         <v>2</v>
@@ -24942,13 +24941,13 @@
         <v>361</v>
       </c>
       <c r="B319" t="s">
+        <v>492</v>
+      </c>
+      <c r="C319" t="s">
         <v>403</v>
       </c>
-      <c r="C319" t="s">
+      <c r="D319" t="s">
         <v>404</v>
-      </c>
-      <c r="D319" t="s">
-        <v>405</v>
       </c>
       <c r="E319">
         <v>1</v>
@@ -24992,13 +24991,13 @@
         <v>361</v>
       </c>
       <c r="B320" t="s">
+        <v>407</v>
+      </c>
+      <c r="C320" t="s">
         <v>408</v>
       </c>
-      <c r="C320" t="s">
+      <c r="D320" t="s">
         <v>409</v>
-      </c>
-      <c r="D320" t="s">
-        <v>410</v>
       </c>
       <c r="E320">
         <v>1</v>
@@ -25007,7 +25006,7 @@
         <v>216</v>
       </c>
       <c r="G320" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H320">
         <v>1</v>
@@ -25019,7 +25018,7 @@
         <v>1</v>
       </c>
       <c r="N320" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P320">
         <v>4</v>
@@ -25045,13 +25044,13 @@
         <v>361</v>
       </c>
       <c r="B321" t="s">
+        <v>407</v>
+      </c>
+      <c r="C321" t="s">
         <v>408</v>
       </c>
-      <c r="C321" t="s">
+      <c r="D321" t="s">
         <v>409</v>
-      </c>
-      <c r="D321" t="s">
-        <v>410</v>
       </c>
       <c r="E321">
         <v>1</v>
@@ -25060,7 +25059,7 @@
         <v>233</v>
       </c>
       <c r="G321" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H321">
         <v>1</v>
@@ -25075,7 +25074,7 @@
         <v>1</v>
       </c>
       <c r="N321" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P321">
         <v>22</v>
@@ -25155,13 +25154,13 @@
         <v>361</v>
       </c>
       <c r="B322" t="s">
+        <v>407</v>
+      </c>
+      <c r="C322" t="s">
         <v>408</v>
       </c>
-      <c r="C322" t="s">
+      <c r="D322" t="s">
         <v>409</v>
-      </c>
-      <c r="D322" t="s">
-        <v>410</v>
       </c>
       <c r="E322">
         <v>1</v>
@@ -25211,13 +25210,13 @@
         <v>361</v>
       </c>
       <c r="B323" t="s">
+        <v>407</v>
+      </c>
+      <c r="C323" t="s">
         <v>408</v>
       </c>
-      <c r="C323" t="s">
+      <c r="D323" t="s">
         <v>409</v>
-      </c>
-      <c r="D323" t="s">
-        <v>410</v>
       </c>
       <c r="E323">
         <v>1</v>
@@ -25258,16 +25257,16 @@
     </row>
     <row r="324" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>411</v>
+      </c>
+      <c r="B324" t="s">
         <v>412</v>
       </c>
-      <c r="B324" t="s">
+      <c r="C324" t="s">
         <v>413</v>
       </c>
-      <c r="C324" t="s">
+      <c r="D324" t="s">
         <v>414</v>
-      </c>
-      <c r="D324" t="s">
-        <v>415</v>
       </c>
       <c r="E324">
         <v>3</v>
@@ -25276,13 +25275,13 @@
         <v>112</v>
       </c>
       <c r="G324" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J324">
         <v>3</v>
       </c>
       <c r="N324" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P324">
         <v>8</v>
@@ -25317,16 +25316,16 @@
     </row>
     <row r="325" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
+        <v>411</v>
+      </c>
+      <c r="B325" t="s">
         <v>412</v>
       </c>
-      <c r="B325" t="s">
+      <c r="C325" t="s">
         <v>413</v>
       </c>
-      <c r="C325" t="s">
+      <c r="D325" t="s">
         <v>414</v>
-      </c>
-      <c r="D325" t="s">
-        <v>415</v>
       </c>
       <c r="E325">
         <v>3</v>
@@ -25335,13 +25334,13 @@
         <v>132</v>
       </c>
       <c r="G325" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J325">
         <v>3</v>
       </c>
       <c r="N325" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P325">
         <v>4</v>
@@ -25364,16 +25363,16 @@
     </row>
     <row r="326" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
+        <v>411</v>
+      </c>
+      <c r="B326" t="s">
         <v>412</v>
       </c>
-      <c r="B326" t="s">
+      <c r="C326" t="s">
         <v>413</v>
       </c>
-      <c r="C326" t="s">
+      <c r="D326" t="s">
         <v>414</v>
-      </c>
-      <c r="D326" t="s">
-        <v>415</v>
       </c>
       <c r="E326">
         <v>4</v>
@@ -25382,7 +25381,7 @@
         <v>251</v>
       </c>
       <c r="G326" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H326">
         <v>3</v>
@@ -25397,7 +25396,7 @@
         <v>3</v>
       </c>
       <c r="N326" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P326">
         <v>4</v>
@@ -25420,16 +25419,16 @@
     </row>
     <row r="327" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>411</v>
+      </c>
+      <c r="B327" t="s">
         <v>412</v>
       </c>
-      <c r="B327" t="s">
+      <c r="C327" t="s">
         <v>413</v>
       </c>
-      <c r="C327" t="s">
+      <c r="D327" t="s">
         <v>414</v>
-      </c>
-      <c r="D327" t="s">
-        <v>415</v>
       </c>
       <c r="E327">
         <v>3</v>
@@ -25438,13 +25437,13 @@
         <v>264</v>
       </c>
       <c r="G327" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K327">
         <v>3</v>
       </c>
       <c r="N327" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P327">
         <v>6</v>
@@ -25473,16 +25472,16 @@
     </row>
     <row r="328" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>411</v>
+      </c>
+      <c r="B328" t="s">
         <v>412</v>
       </c>
-      <c r="B328" t="s">
+      <c r="C328" t="s">
         <v>413</v>
       </c>
-      <c r="C328" t="s">
+      <c r="D328" t="s">
         <v>414</v>
-      </c>
-      <c r="D328" t="s">
-        <v>415</v>
       </c>
       <c r="E328">
         <v>3</v>
@@ -25523,16 +25522,16 @@
     </row>
     <row r="329" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>411</v>
+      </c>
+      <c r="B329" t="s">
         <v>412</v>
       </c>
-      <c r="B329" t="s">
+      <c r="C329" t="s">
         <v>413</v>
       </c>
-      <c r="C329" t="s">
+      <c r="D329" t="s">
         <v>414</v>
-      </c>
-      <c r="D329" t="s">
-        <v>415</v>
       </c>
       <c r="E329">
         <v>3</v>
@@ -25567,16 +25566,16 @@
     </row>
     <row r="330" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
+        <v>411</v>
+      </c>
+      <c r="B330" t="s">
         <v>412</v>
       </c>
-      <c r="B330" t="s">
+      <c r="C330" t="s">
         <v>413</v>
       </c>
-      <c r="C330" t="s">
+      <c r="D330" t="s">
         <v>414</v>
-      </c>
-      <c r="D330" t="s">
-        <v>415</v>
       </c>
       <c r="E330">
         <v>3</v>
@@ -25585,7 +25584,7 @@
         <v>254</v>
       </c>
       <c r="G330" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H330">
         <v>3</v>
@@ -25600,7 +25599,7 @@
         <v>3</v>
       </c>
       <c r="N330" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P330">
         <v>2</v>
@@ -25617,25 +25616,25 @@
     </row>
     <row r="331" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
+        <v>411</v>
+      </c>
+      <c r="B331" t="s">
         <v>412</v>
       </c>
-      <c r="B331" t="s">
+      <c r="C331" t="s">
         <v>413</v>
       </c>
-      <c r="C331" t="s">
+      <c r="D331" t="s">
         <v>414</v>
-      </c>
-      <c r="D331" t="s">
-        <v>415</v>
       </c>
       <c r="E331">
         <v>3</v>
       </c>
       <c r="F331" t="s">
+        <v>422</v>
+      </c>
+      <c r="G331" t="s">
         <v>423</v>
-      </c>
-      <c r="G331" t="s">
-        <v>424</v>
       </c>
       <c r="H331">
         <v>3</v>
@@ -25667,16 +25666,16 @@
     </row>
     <row r="332" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B332" t="s">
+        <v>424</v>
+      </c>
+      <c r="C332" t="s">
         <v>425</v>
       </c>
-      <c r="C332" t="s">
+      <c r="D332" t="s">
         <v>426</v>
-      </c>
-      <c r="D332" t="s">
-        <v>427</v>
       </c>
       <c r="E332">
         <v>2</v>
@@ -25685,13 +25684,13 @@
         <v>216</v>
       </c>
       <c r="G332" t="s">
+        <v>427</v>
+      </c>
+      <c r="I332">
+        <v>1</v>
+      </c>
+      <c r="N332" t="s">
         <v>428</v>
-      </c>
-      <c r="I332">
-        <v>1</v>
-      </c>
-      <c r="N332" t="s">
-        <v>429</v>
       </c>
       <c r="P332">
         <v>10</v>
@@ -25732,16 +25731,16 @@
     </row>
     <row r="333" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B333" t="s">
+        <v>424</v>
+      </c>
+      <c r="C333" t="s">
         <v>425</v>
       </c>
-      <c r="C333" t="s">
+      <c r="D333" t="s">
         <v>426</v>
-      </c>
-      <c r="D333" t="s">
-        <v>427</v>
       </c>
       <c r="E333">
         <v>2</v>
@@ -25750,13 +25749,13 @@
         <v>269</v>
       </c>
       <c r="G333" t="s">
+        <v>429</v>
+      </c>
+      <c r="I333">
+        <v>1</v>
+      </c>
+      <c r="N333" t="s">
         <v>430</v>
-      </c>
-      <c r="I333">
-        <v>1</v>
-      </c>
-      <c r="N333" t="s">
-        <v>431</v>
       </c>
       <c r="P333">
         <v>8</v>
@@ -25791,16 +25790,16 @@
     </row>
     <row r="334" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B334" t="s">
+        <v>424</v>
+      </c>
+      <c r="C334" t="s">
         <v>425</v>
       </c>
-      <c r="C334" t="s">
+      <c r="D334" t="s">
         <v>426</v>
-      </c>
-      <c r="D334" t="s">
-        <v>427</v>
       </c>
       <c r="E334">
         <v>2</v>
@@ -25809,13 +25808,13 @@
         <v>107</v>
       </c>
       <c r="G334" t="s">
+        <v>431</v>
+      </c>
+      <c r="K334">
+        <v>1</v>
+      </c>
+      <c r="N334" t="s">
         <v>432</v>
-      </c>
-      <c r="K334">
-        <v>1</v>
-      </c>
-      <c r="N334" t="s">
-        <v>433</v>
       </c>
       <c r="P334">
         <v>4</v>
@@ -25838,16 +25837,16 @@
     </row>
     <row r="335" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B335" t="s">
+        <v>424</v>
+      </c>
+      <c r="C335" t="s">
         <v>425</v>
       </c>
-      <c r="C335" t="s">
+      <c r="D335" t="s">
         <v>426</v>
-      </c>
-      <c r="D335" t="s">
-        <v>427</v>
       </c>
       <c r="E335">
         <v>2</v>
@@ -25856,7 +25855,7 @@
         <v>359</v>
       </c>
       <c r="G335" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K335">
         <v>1</v>
@@ -25865,7 +25864,7 @@
         <v>1</v>
       </c>
       <c r="N335" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P335">
         <v>4</v>
@@ -25888,16 +25887,16 @@
     </row>
     <row r="336" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B336" t="s">
+        <v>424</v>
+      </c>
+      <c r="C336" t="s">
         <v>425</v>
       </c>
-      <c r="C336" t="s">
+      <c r="D336" t="s">
         <v>426</v>
-      </c>
-      <c r="D336" t="s">
-        <v>427</v>
       </c>
       <c r="E336">
         <v>2</v>
@@ -25906,7 +25905,7 @@
         <v>174</v>
       </c>
       <c r="G336" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H336">
         <v>1</v>
@@ -25929,16 +25928,16 @@
     </row>
     <row r="337" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B337" t="s">
+        <v>424</v>
+      </c>
+      <c r="C337" t="s">
         <v>425</v>
       </c>
-      <c r="C337" t="s">
+      <c r="D337" t="s">
         <v>426</v>
-      </c>
-      <c r="D337" t="s">
-        <v>427</v>
       </c>
       <c r="E337">
         <v>2</v>
@@ -25947,7 +25946,7 @@
         <v>124</v>
       </c>
       <c r="G337" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J337">
         <v>1</v>
@@ -25956,7 +25955,7 @@
         <v>1</v>
       </c>
       <c r="N337" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P337">
         <v>2</v>
@@ -25973,16 +25972,16 @@
     </row>
     <row r="338" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B338" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C338" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D338" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E338">
         <v>6</v>
@@ -25991,7 +25990,7 @@
         <v>248</v>
       </c>
       <c r="G338" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H338">
         <v>1</v>
@@ -26006,7 +26005,7 @@
         <v>1</v>
       </c>
       <c r="N338" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P338">
         <v>10</v>
@@ -26047,16 +26046,16 @@
     </row>
     <row r="339" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B339" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C339" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D339" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E339">
         <v>6</v>
@@ -26065,7 +26064,7 @@
         <v>231</v>
       </c>
       <c r="G339" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I339">
         <v>1</v>
@@ -26077,7 +26076,7 @@
         <v>1</v>
       </c>
       <c r="N339" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P339">
         <v>8</v>
@@ -26112,16 +26111,16 @@
     </row>
     <row r="340" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B340" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C340" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D340" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E340">
         <v>6</v>
@@ -26130,13 +26129,13 @@
         <v>233</v>
       </c>
       <c r="G340" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H340">
         <v>1</v>
       </c>
       <c r="N340" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P340">
         <v>10</v>
@@ -26177,16 +26176,16 @@
     </row>
     <row r="341" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B341" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C341" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D341" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E341">
         <v>6</v>
@@ -26195,7 +26194,7 @@
         <v>181</v>
       </c>
       <c r="G341" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L341">
         <v>1</v>
@@ -26221,16 +26220,16 @@
     </row>
     <row r="342" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B342" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C342" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D342" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E342">
         <v>5</v>
@@ -26239,13 +26238,13 @@
         <v>210</v>
       </c>
       <c r="G342" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K342">
         <v>1</v>
       </c>
       <c r="N342" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P342">
         <v>8</v>
@@ -26280,16 +26279,16 @@
     </row>
     <row r="343" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B343" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C343" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D343" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E343">
         <v>5</v>
@@ -26298,13 +26297,13 @@
         <v>310</v>
       </c>
       <c r="G343" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H343">
         <v>1</v>
       </c>
       <c r="N343" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P343">
         <v>10</v>
@@ -26345,16 +26344,16 @@
     </row>
     <row r="344" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B344" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C344" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D344" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E344">
         <v>5</v>
@@ -26363,13 +26362,13 @@
         <v>143</v>
       </c>
       <c r="G344" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H344">
         <v>1</v>
       </c>
       <c r="N344" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P344">
         <v>10</v>
@@ -26410,16 +26409,16 @@
     </row>
     <row r="345" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B345" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C345" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D345" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E345">
         <v>5</v>
@@ -26428,7 +26427,7 @@
         <v>181</v>
       </c>
       <c r="G345" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L345">
         <v>1</v>
@@ -26451,31 +26450,31 @@
     </row>
     <row r="346" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B346" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C346" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D346" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E346">
         <v>4</v>
       </c>
       <c r="F346" t="s">
+        <v>446</v>
+      </c>
+      <c r="G346" t="s">
         <v>447</v>
       </c>
-      <c r="G346" t="s">
-        <v>448</v>
-      </c>
       <c r="J346">
         <v>1</v>
       </c>
       <c r="N346" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P346">
         <v>10</v>
@@ -26516,16 +26515,16 @@
     </row>
     <row r="347" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B347" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C347" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D347" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E347">
         <v>4</v>
@@ -26534,13 +26533,13 @@
         <v>207</v>
       </c>
       <c r="G347" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J347">
         <v>1</v>
       </c>
       <c r="N347" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P347">
         <v>8</v>
@@ -26575,16 +26574,16 @@
     </row>
     <row r="348" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B348" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C348" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D348" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E348">
         <v>4</v>
@@ -26593,13 +26592,13 @@
         <v>121</v>
       </c>
       <c r="G348" t="s">
+        <v>449</v>
+      </c>
+      <c r="H348">
+        <v>1</v>
+      </c>
+      <c r="N348" t="s">
         <v>450</v>
-      </c>
-      <c r="H348">
-        <v>1</v>
-      </c>
-      <c r="N348" t="s">
-        <v>451</v>
       </c>
       <c r="P348">
         <v>8</v>
@@ -26634,16 +26633,16 @@
     </row>
     <row r="349" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B349" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C349" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D349" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E349">
         <v>4</v>
@@ -26652,7 +26651,7 @@
         <v>137</v>
       </c>
       <c r="G349" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L349">
         <v>1</v>
@@ -26675,16 +26674,16 @@
     </row>
     <row r="350" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B350" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C350" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D350" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E350">
         <v>4</v>
@@ -26693,7 +26692,7 @@
         <v>181</v>
       </c>
       <c r="G350" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L350">
         <v>1</v>
@@ -26716,16 +26715,16 @@
     </row>
     <row r="351" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B351" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C351" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D351" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E351">
         <v>5</v>
@@ -26734,13 +26733,13 @@
         <v>210</v>
       </c>
       <c r="G351" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K351">
         <v>1</v>
       </c>
       <c r="N351" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P351">
         <v>8</v>
@@ -26775,16 +26774,16 @@
     </row>
     <row r="352" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B352" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C352" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D352" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E352">
         <v>5</v>
@@ -26793,13 +26792,13 @@
         <v>310</v>
       </c>
       <c r="G352" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H352">
         <v>1</v>
       </c>
       <c r="N352" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P352">
         <v>4</v>
@@ -26822,16 +26821,16 @@
     </row>
     <row r="353" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B353" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C353" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D353" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E353">
         <v>5</v>
@@ -26840,13 +26839,13 @@
         <v>328</v>
       </c>
       <c r="G353" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H353">
         <v>1</v>
       </c>
       <c r="N353" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P353">
         <v>4</v>
@@ -26869,16 +26868,16 @@
     </row>
     <row r="354" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B354" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C354" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D354" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E354">
         <v>5</v>
@@ -26887,13 +26886,13 @@
         <v>143</v>
       </c>
       <c r="G354" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H354">
         <v>1</v>
       </c>
       <c r="N354" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P354">
         <v>10</v>
@@ -26934,16 +26933,16 @@
     </row>
     <row r="355" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B355" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C355" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D355" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E355">
         <v>5</v>
@@ -26952,13 +26951,13 @@
         <v>181</v>
       </c>
       <c r="G355" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L355">
         <v>1</v>
       </c>
       <c r="N355" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P355">
         <v>2</v>
@@ -26975,16 +26974,16 @@
     </row>
     <row r="356" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B356" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C356" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D356" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E356">
         <v>5</v>
@@ -26993,13 +26992,13 @@
         <v>163</v>
       </c>
       <c r="G356" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J356">
         <v>1</v>
       </c>
       <c r="N356" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P356">
         <v>2</v>
@@ -27016,16 +27015,16 @@
     </row>
     <row r="357" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B357" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C357" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D357" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E357">
         <v>1</v>
@@ -27034,13 +27033,13 @@
         <v>110</v>
       </c>
       <c r="G357" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I357">
         <v>1</v>
       </c>
       <c r="N357" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P357">
         <v>10</v>
@@ -27081,16 +27080,16 @@
     </row>
     <row r="358" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B358" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C358" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D358" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E358">
         <v>1</v>
@@ -27099,13 +27098,13 @@
         <v>272</v>
       </c>
       <c r="G358" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M358">
         <v>1</v>
       </c>
       <c r="N358" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P358">
         <v>8</v>
@@ -27140,16 +27139,16 @@
     </row>
     <row r="359" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B359" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C359" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D359" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E359">
         <v>1</v>
@@ -27158,7 +27157,7 @@
         <v>179</v>
       </c>
       <c r="G359" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H359">
         <v>1</v>
@@ -27173,7 +27172,7 @@
         <v>1</v>
       </c>
       <c r="N359" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P359">
         <v>8</v>
@@ -27208,16 +27207,16 @@
     </row>
     <row r="360" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B360" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C360" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D360" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E360">
         <v>1</v>
@@ -27226,7 +27225,7 @@
         <v>124</v>
       </c>
       <c r="G360" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H360">
         <v>1</v>
@@ -27252,16 +27251,16 @@
     </row>
     <row r="361" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B361" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C361" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D361" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E361">
         <v>1</v>
@@ -27270,13 +27269,13 @@
         <v>115</v>
       </c>
       <c r="G361" t="s">
+        <v>460</v>
+      </c>
+      <c r="I361">
+        <v>1</v>
+      </c>
+      <c r="N361" t="s">
         <v>461</v>
-      </c>
-      <c r="I361">
-        <v>1</v>
-      </c>
-      <c r="N361" t="s">
-        <v>462</v>
       </c>
       <c r="P361">
         <v>2</v>
@@ -27293,31 +27292,31 @@
     </row>
     <row r="362" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B362" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C362" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D362" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E362">
         <v>4</v>
       </c>
       <c r="F362" t="s">
+        <v>446</v>
+      </c>
+      <c r="G362" t="s">
         <v>447</v>
       </c>
-      <c r="G362" t="s">
-        <v>448</v>
-      </c>
       <c r="J362">
         <v>1</v>
       </c>
       <c r="N362" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P362">
         <v>8</v>
@@ -27352,16 +27351,16 @@
     </row>
     <row r="363" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B363" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C363" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D363" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E363">
         <v>4</v>
@@ -27370,13 +27369,13 @@
         <v>207</v>
       </c>
       <c r="G363" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J363">
         <v>1</v>
       </c>
       <c r="N363" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P363">
         <v>10</v>
@@ -27417,16 +27416,16 @@
     </row>
     <row r="364" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B364" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C364" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D364" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E364">
         <v>4</v>
@@ -27435,13 +27434,13 @@
         <v>121</v>
       </c>
       <c r="G364" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H364">
         <v>1</v>
       </c>
       <c r="N364" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P364">
         <v>8</v>
@@ -27476,16 +27475,16 @@
     </row>
     <row r="365" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B365" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C365" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D365" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E365">
         <v>4</v>
@@ -27494,7 +27493,7 @@
         <v>137</v>
       </c>
       <c r="G365" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L365">
         <v>1</v>
@@ -27517,16 +27516,16 @@
     </row>
     <row r="366" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B366" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C366" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D366" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E366">
         <v>4</v>
@@ -27535,7 +27534,7 @@
         <v>181</v>
       </c>
       <c r="G366" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K366">
         <v>1</v>
@@ -27558,16 +27557,16 @@
     </row>
     <row r="367" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B367" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C367" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D367" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E367">
         <v>1</v>
@@ -27576,7 +27575,7 @@
         <v>179</v>
       </c>
       <c r="G367" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H367">
         <v>1</v>
@@ -27591,7 +27590,7 @@
         <v>1</v>
       </c>
       <c r="N367" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P367">
         <v>8</v>
@@ -27626,16 +27625,16 @@
     </row>
     <row r="368" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B368" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C368" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D368" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E368">
         <v>1</v>
@@ -27644,13 +27643,13 @@
         <v>272</v>
       </c>
       <c r="G368" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M368">
         <v>1</v>
       </c>
       <c r="N368" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P368">
         <v>8</v>
@@ -27685,16 +27684,16 @@
     </row>
     <row r="369" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B369" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C369" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D369" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E369">
         <v>1</v>
@@ -27703,13 +27702,13 @@
         <v>110</v>
       </c>
       <c r="G369" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I369">
         <v>1</v>
       </c>
       <c r="N369" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P369">
         <v>10</v>
@@ -27750,16 +27749,16 @@
     </row>
     <row r="370" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B370" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C370" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D370" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E370">
         <v>1</v>
@@ -27768,13 +27767,13 @@
         <v>115</v>
       </c>
       <c r="G370" t="s">
+        <v>460</v>
+      </c>
+      <c r="I370">
+        <v>1</v>
+      </c>
+      <c r="N370" t="s">
         <v>461</v>
-      </c>
-      <c r="I370">
-        <v>1</v>
-      </c>
-      <c r="N370" t="s">
-        <v>462</v>
       </c>
       <c r="P370">
         <v>2</v>
@@ -27791,16 +27790,16 @@
     </row>
     <row r="371" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B371" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C371" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D371" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E371">
         <v>1</v>
@@ -27809,7 +27808,7 @@
         <v>124</v>
       </c>
       <c r="G371" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H371">
         <v>1</v>
@@ -27835,16 +27834,16 @@
     </row>
     <row r="372" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B372" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C372" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D372" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E372">
         <v>1</v>
@@ -27853,16 +27852,16 @@
         <v>110</v>
       </c>
       <c r="G372" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I372">
         <v>1</v>
       </c>
       <c r="N372" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P372">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q372">
         <v>96</v>
@@ -27891,19 +27890,25 @@
       <c r="BU372">
         <v>1004</v>
       </c>
+      <c r="CN372">
+        <v>1004</v>
+      </c>
+      <c r="CO372">
+        <v>1004</v>
+      </c>
     </row>
     <row r="373" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B373" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C373" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D373" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E373">
         <v>1</v>
@@ -27912,13 +27917,13 @@
         <v>272</v>
       </c>
       <c r="G373" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M373">
         <v>1</v>
       </c>
       <c r="N373" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P373">
         <v>8</v>
@@ -27953,16 +27958,16 @@
     </row>
     <row r="374" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B374" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C374" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D374" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E374">
         <v>1</v>
@@ -27971,7 +27976,7 @@
         <v>179</v>
       </c>
       <c r="G374" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H374">
         <v>1</v>
@@ -27986,7 +27991,7 @@
         <v>1</v>
       </c>
       <c r="N374" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P374">
         <v>6</v>
@@ -28015,16 +28020,16 @@
     </row>
     <row r="375" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B375" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C375" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D375" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E375">
         <v>1</v>
@@ -28033,13 +28038,13 @@
         <v>115</v>
       </c>
       <c r="G375" t="s">
+        <v>460</v>
+      </c>
+      <c r="J375">
+        <v>1</v>
+      </c>
+      <c r="N375" t="s">
         <v>461</v>
-      </c>
-      <c r="J375">
-        <v>1</v>
-      </c>
-      <c r="N375" t="s">
-        <v>462</v>
       </c>
       <c r="P375">
         <v>2</v>
@@ -28056,16 +28061,16 @@
     </row>
     <row r="376" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B376" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C376" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D376" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E376">
         <v>1</v>
@@ -28074,7 +28079,7 @@
         <v>174</v>
       </c>
       <c r="G376" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I376">
         <v>1</v>
@@ -28097,16 +28102,16 @@
     </row>
     <row r="377" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B377" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C377" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D377" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E377">
         <v>1</v>
@@ -28115,7 +28120,7 @@
         <v>124</v>
       </c>
       <c r="G377" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H377">
         <v>1</v>
@@ -28124,7 +28129,7 @@
         <v>1</v>
       </c>
       <c r="N377" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P377">
         <v>2</v>
@@ -28438,11 +28443,11 @@
       </c>
       <c r="CN378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[16-17V])</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CO378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[17-18V])</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CP378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[18-19V])</f>
@@ -28546,10 +28551,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -28586,7 +28591,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -28602,7 +28607,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B10">
         <v>34</v>
@@ -28618,7 +28623,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B12">
         <v>30</v>
@@ -28634,7 +28639,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B14">
         <v>26</v>
@@ -28650,7 +28655,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B16">
         <v>18</v>
@@ -28666,7 +28671,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B18">
         <v>14</v>
@@ -28682,7 +28687,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -28690,7 +28695,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B21">
         <v>34</v>
@@ -28698,7 +28703,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B22">
         <v>32</v>
@@ -28730,7 +28735,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -28738,7 +28743,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B27">
         <v>24</v>
@@ -28746,7 +28751,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B28">
         <v>24</v>
@@ -28754,7 +28759,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B29">
         <v>25</v>
@@ -28768,10 +28773,10 @@
         <v>24</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E30" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -28796,7 +28801,7 @@
         <v>36</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -28810,7 +28815,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E33">
         <v>9</v>
@@ -28838,7 +28843,7 @@
         <v>28</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -28916,13 +28921,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B41">
         <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -29006,7 +29011,7 @@
         <v>22</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E47">
         <v>69</v>
@@ -29046,7 +29051,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B52">
         <v>22</v>
@@ -29054,7 +29059,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B53">
         <v>38</v>
@@ -29118,7 +29123,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B61">
         <v>26</v>
@@ -29126,7 +29131,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B62">
         <v>22</v>
@@ -29158,7 +29163,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B66">
         <v>26</v>
@@ -29174,7 +29179,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B68">
         <v>30</v>
@@ -29182,7 +29187,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -29222,7 +29227,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B74">
         <v>34</v>
@@ -29246,7 +29251,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B77">
         <v>26</v>
@@ -29286,7 +29291,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B82">
         <v>2042</v>

</xml_diff>

<commit_message>
Update INSTRUCTOR field in horarios/1-2024.json
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024.xlsx
+++ b/static/horarios/1-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3532FC2-44B5-47F2-973C-D5F33484A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3434D68-7BBF-4DE4-8F73-0BF1C76F9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$378</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -106,7 +106,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="504">
   <si>
     <t>Source.Name</t>
   </si>
@@ -1624,6 +1624,9 @@
   </si>
   <si>
     <t>2903769 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yorman Andrés Calderón Yepes</t>
   </si>
 </sst>
 </file>
@@ -1715,14 +1718,7 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1746,7 +1742,14 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7570,893 +7573,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C494C86E-4DC1-488C-A314-1E315242265A}" name="PivotChartTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="78">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="72"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="75"/>
-        <item x="76"/>
-        <item x="77"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="79">
-    <i>
-      <x v="62"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="69"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="63"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="71"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="75"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="67"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="65"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="68"/>
-    </i>
-    <i>
-      <x v="76"/>
-    </i>
-    <i>
-      <x v="70"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="73"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="66"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="72"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="77"/>
-    </i>
-    <i>
-      <x v="74"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="64"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de HORAS SEMANAL" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="111">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="13"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
-      <x15:pivotTableData rowCount="79" columnCount="1" cacheId="531005254">
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>38</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>38</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>34</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>34</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>32</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>32</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>31</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>23</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>23</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>18</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>18</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>14</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>12</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>10</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2044</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-      </x15:pivotTableData>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
-        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1864DD7E-914F-4129-81BE-DE6895877F42}" name="PivotChartTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:I19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -9254,6 +8370,893 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C494C86E-4DC1-488C-A314-1E315242265A}" name="PivotChartTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="78">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="79">
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de HORAS SEMANAL" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="111">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="13"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
+      <x15:pivotTableData rowCount="79" columnCount="1" cacheId="531005254">
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>38</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>38</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>34</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>34</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>32</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>32</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>31</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>23</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>23</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>18</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>18</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>14</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>12</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>10</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2044</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+      </x15:pivotTableData>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
+        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E51D2C13-18A8-44E4-9514-17D00C659F63}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B82" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
@@ -10123,21 +10126,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}" name="PROGRAMACIONES_PARCIALES" displayName="PROGRAMACIONES_PARCIALES" ref="A2:DI379" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A2:DI378" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}"/>
   <tableColumns count="113">
-    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{8B226D1B-BFF2-49BB-B758-EE4B851E70DA}" uniqueName="5" name="TRIMESTRE ACADÉMICO" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE DE LA COMPETENCIA" queryTableFieldId="7" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE DE LA COMPETENCIA" queryTableFieldId="7" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{5C00E006-DEB8-4B45-B7E3-B775FAC56914}" uniqueName="8" name="RAP 1" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{49EFD39C-728B-4C81-8193-D20CD8923D69}" uniqueName="9" name="RAP 2" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{B6F8F457-5381-4426-9F22-D87B3BAE1E1B}" uniqueName="10" name="RAP 3" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0EECA1C3-E5FD-4979-BEEB-1A297BEFAD06}" uniqueName="11" name="RAP 4" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{D0A977BB-7A27-4EF0-B307-4BAD18A1D841}" uniqueName="12" name="RAP 5" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{F8C8EBB1-C23A-49D5-B16B-0380006A1DDD}" uniqueName="13" name="RAP 6" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="0"/>
     <tableColumn id="16" xr3:uid="{34761CDE-83A0-4FFA-B1E9-1FEBE9DC1075}" uniqueName="16" name="HORAS SEMANAL" queryTableFieldId="16"/>
     <tableColumn id="17" xr3:uid="{B25F73F1-9F14-47B9-B123-7A878796CCA7}" uniqueName="17" name="HORAS POR TRIMESTRE" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{3F05A4C2-F912-4CB3-AA16-A7656C50765A}" uniqueName="18" name="6-7L" totalsRowFunction="custom" queryTableFieldId="18">
@@ -10700,8 +10703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C46E5B-3CE7-4F67-9F7E-3BDF34AAB992}">
   <dimension ref="A1:DI379"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:DI378"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N378" sqref="N378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11789,7 +11792,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -12609,7 +12612,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P25">
         <v>2</v>
@@ -14204,7 +14207,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P53">
         <v>2</v>
@@ -16210,7 +16213,7 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P87">
         <v>2</v>
@@ -17123,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O104" t="s">
         <v>195</v>
@@ -19840,7 +19843,7 @@
         <v>1</v>
       </c>
       <c r="N153" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O153" t="s">
         <v>195</v>
@@ -20436,7 +20439,7 @@
         <v>1</v>
       </c>
       <c r="N163" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O163" t="s">
         <v>195</v>
@@ -22308,7 +22311,7 @@
         <v>1</v>
       </c>
       <c r="N196" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O196" t="s">
         <v>195</v>
@@ -22682,7 +22685,7 @@
         <v>1</v>
       </c>
       <c r="N203" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O203" t="s">
         <v>195</v>
@@ -23371,7 +23374,7 @@
         <v>1</v>
       </c>
       <c r="N216" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="O216" t="s">
         <v>195</v>
@@ -24857,7 +24860,7 @@
         <v>1</v>
       </c>
       <c r="N242" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P242">
         <v>2</v>
@@ -26355,7 +26358,7 @@
         <v>1</v>
       </c>
       <c r="N271" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P271">
         <v>2</v>
@@ -27239,7 +27242,7 @@
         <v>1</v>
       </c>
       <c r="N287" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P287">
         <v>2</v>
@@ -30278,7 +30281,7 @@
         <v>1</v>
       </c>
       <c r="N338" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P338">
         <v>2</v>
@@ -31280,7 +31283,7 @@
         <v>1</v>
       </c>
       <c r="N356" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P356">
         <v>2</v>
@@ -32452,7 +32455,7 @@
         <v>1</v>
       </c>
       <c r="N378" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="P378">
         <v>2</v>
@@ -32846,7 +32849,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R379:DA379">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update compiled Python file and Excel file
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024.xlsx
+++ b/static/horarios/1-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3434D68-7BBF-4DE4-8F73-0BF1C76F9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0021555C-C2E0-4A32-B210-BE937505148C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$378</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -106,7 +106,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1626,7 +1626,7 @@
     <t>2903769 C</t>
   </si>
   <si>
-    <t xml:space="preserve"> Yorman Andrés Calderón Yepes</t>
+    <t>YORMAN ANDRÉS CALDERÓN YEPES</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1718,14 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1742,14 +1749,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10126,21 +10126,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}" name="PROGRAMACIONES_PARCIALES" displayName="PROGRAMACIONES_PARCIALES" ref="A2:DI379" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A2:DI378" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}"/>
   <tableColumns count="113">
-    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{8B226D1B-BFF2-49BB-B758-EE4B851E70DA}" uniqueName="5" name="TRIMESTRE ACADÉMICO" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE DE LA COMPETENCIA" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE DE LA COMPETENCIA" queryTableFieldId="7" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{5C00E006-DEB8-4B45-B7E3-B775FAC56914}" uniqueName="8" name="RAP 1" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{49EFD39C-728B-4C81-8193-D20CD8923D69}" uniqueName="9" name="RAP 2" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{B6F8F457-5381-4426-9F22-D87B3BAE1E1B}" uniqueName="10" name="RAP 3" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0EECA1C3-E5FD-4979-BEEB-1A297BEFAD06}" uniqueName="11" name="RAP 4" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{D0A977BB-7A27-4EF0-B307-4BAD18A1D841}" uniqueName="12" name="RAP 5" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{F8C8EBB1-C23A-49D5-B16B-0380006A1DDD}" uniqueName="13" name="RAP 6" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{34761CDE-83A0-4FFA-B1E9-1FEBE9DC1075}" uniqueName="16" name="HORAS SEMANAL" queryTableFieldId="16"/>
     <tableColumn id="17" xr3:uid="{B25F73F1-9F14-47B9-B123-7A878796CCA7}" uniqueName="17" name="HORAS POR TRIMESTRE" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{3F05A4C2-F912-4CB3-AA16-A7656C50765A}" uniqueName="18" name="6-7L" totalsRowFunction="custom" queryTableFieldId="18">
@@ -10704,7 +10704,7 @@
   <dimension ref="A1:DI379"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N378" sqref="N378"/>
+      <selection activeCell="N203" sqref="N203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32849,7 +32849,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R379:DA379">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update instructor names in course schedule
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024.xlsx
+++ b/static/horarios/1-2024.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sena\Desktop\schedule\static\horarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E85A19-F965-43A9-A76F-E2FA1A057C44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73D35C-A80E-4B59-B26B-330838CAE445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROGRAMACIÓN I 2024" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$378</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -104,7 +104,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="508">
   <si>
     <t>Source.Name</t>
   </si>
@@ -1634,6 +1634,9 @@
   </si>
   <si>
     <t>HORAS_SEMANAL</t>
+  </si>
+  <si>
+    <t>JANER ALFONSO PAREJA GUTIERREZ</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1728,14 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1749,14 +1759,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1811,7 +1814,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1859,7 +1862,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2435,7 +2438,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="533591440"/>
@@ -2499,7 +2502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1267078032"/>
@@ -2546,7 +2549,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2583,9 +2586,14 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
@@ -2667,7 +2675,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3938,7 +3946,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3994,7 +4002,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4050,7 +4058,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4106,7 +4114,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4162,7 +4170,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4218,7 +4226,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4274,7 +4282,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -5038,7 +5046,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1835362880"/>
@@ -5102,7 +5110,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1089398640"/>
@@ -5149,7 +5157,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5186,9 +5194,14 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
@@ -10123,21 +10136,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}" name="PROGRAMACIONES_PARCIALES" displayName="PROGRAMACIONES_PARCIALES" ref="A2:DI379" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A2:DI378" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}"/>
   <tableColumns count="113">
-    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{8B226D1B-BFF2-49BB-B758-EE4B851E70DA}" uniqueName="5" name="TRIMESTRE_ACADÉMICO" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE_COMPETENCIA" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE_COMPETENCIA" queryTableFieldId="7" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{5C00E006-DEB8-4B45-B7E3-B775FAC56914}" uniqueName="8" name="RAP 1" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{49EFD39C-728B-4C81-8193-D20CD8923D69}" uniqueName="9" name="RAP 2" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{B6F8F457-5381-4426-9F22-D87B3BAE1E1B}" uniqueName="10" name="RAP 3" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0EECA1C3-E5FD-4979-BEEB-1A297BEFAD06}" uniqueName="11" name="RAP 4" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{D0A977BB-7A27-4EF0-B307-4BAD18A1D841}" uniqueName="12" name="RAP 5" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{F8C8EBB1-C23A-49D5-B16B-0380006A1DDD}" uniqueName="13" name="RAP 6" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{34761CDE-83A0-4FFA-B1E9-1FEBE9DC1075}" uniqueName="16" name="HORAS_SEMANAL" queryTableFieldId="16"/>
     <tableColumn id="17" xr3:uid="{B25F73F1-9F14-47B9-B123-7A878796CCA7}" uniqueName="17" name="HORAS POR TRIMESTRE" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{3F05A4C2-F912-4CB3-AA16-A7656C50765A}" uniqueName="18" name="6-7L" totalsRowFunction="custom" queryTableFieldId="18">
@@ -10678,7 +10691,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -10701,45 +10714,45 @@
   <dimension ref="A1:DI379"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="81.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="81.109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24" hidden="1" customWidth="1"/>
-    <col min="18" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="33" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="49" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="65" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="81" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="82" max="84" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="86" max="97" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="9.28515625" customWidth="1"/>
+    <col min="18" max="20" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="33" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="49" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="65" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="81" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="84" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="97" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.33203125" customWidth="1"/>
     <col min="99" max="100" width="7" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="8" bestFit="1" customWidth="1"/>
     <col min="102" max="105" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:113" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P1" s="1">
         <f>SUBTOTAL(9,PROGRAMACIONES_PARCIALES[HORAS_SEMANAL])</f>
         <v>2038</v>
@@ -10845,7 +10858,7 @@
       <c r="CZ1" s="6"/>
       <c r="DA1" s="6"/>
     </row>
-    <row r="2" spans="1:113" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:113" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -11186,7 +11199,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -11251,7 +11264,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -11337,7 +11350,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -11387,7 +11400,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -11428,7 +11441,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -11550,7 +11563,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="8" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -11600,7 +11613,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="9" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -11641,7 +11654,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="10" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -11763,7 +11776,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -11804,7 +11817,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="12" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -11869,7 +11882,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -11955,7 +11968,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -12005,7 +12018,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -12046,7 +12059,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -12156,7 +12169,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -12206,7 +12219,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -12256,7 +12269,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -12297,7 +12310,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -12383,7 +12396,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="21" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -12433,7 +12446,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="22" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -12483,7 +12496,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="23" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -12533,7 +12546,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="24" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -12583,7 +12596,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="25" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -12624,7 +12637,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="26" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -12728,7 +12741,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="27" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -12778,7 +12791,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -12828,7 +12841,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -12878,7 +12891,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -12919,7 +12932,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -13005,7 +13018,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="32" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -13055,7 +13068,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="33" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -13105,7 +13118,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -13155,7 +13168,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="35" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -13205,7 +13218,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="36" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -13246,7 +13259,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="37" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -13344,7 +13357,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="38" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -13394,7 +13407,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="39" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -13444,7 +13457,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="40" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -13494,7 +13507,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="41" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -13544,7 +13557,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="42" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -13585,7 +13598,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="43" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -13683,7 +13696,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="44" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -13733,7 +13746,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="45" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -13783,7 +13796,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="46" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -13833,7 +13846,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="47" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -13883,7 +13896,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="48" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -13924,7 +13937,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="49" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -14028,7 +14041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -14078,7 +14091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -14128,7 +14141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -14178,7 +14191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -14219,7 +14232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -14335,7 +14348,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="55" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -14385,7 +14398,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="56" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>100</v>
       </c>
@@ -14426,7 +14439,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="57" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -14485,7 +14498,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="58" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -14559,7 +14572,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="59" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -14609,7 +14622,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="60" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -14659,7 +14672,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="61" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>100</v>
       </c>
@@ -14709,7 +14722,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="62" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>100</v>
       </c>
@@ -14759,7 +14772,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="63" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>100</v>
       </c>
@@ -14800,7 +14813,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="64" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>100</v>
       </c>
@@ -14832,7 +14845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -14930,7 +14943,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="66" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>100</v>
       </c>
@@ -14980,7 +14993,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="67" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>100</v>
       </c>
@@ -15030,7 +15043,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="68" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -15080,7 +15093,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="69" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>100</v>
       </c>
@@ -15121,7 +15134,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="70" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>100</v>
       </c>
@@ -15165,7 +15178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>100</v>
       </c>
@@ -15281,7 +15294,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="72" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -15331,7 +15344,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="73" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>100</v>
       </c>
@@ -15381,7 +15394,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="74" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>100</v>
       </c>
@@ -15422,7 +15435,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="75" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>100</v>
       </c>
@@ -15466,7 +15479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>100</v>
       </c>
@@ -15582,7 +15595,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="77" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>100</v>
       </c>
@@ -15632,7 +15645,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="78" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>100</v>
       </c>
@@ -15682,7 +15695,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="79" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>100</v>
       </c>
@@ -15723,7 +15736,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="80" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -15767,7 +15780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -15889,7 +15902,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="82" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -15930,7 +15943,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="83" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -15980,7 +15993,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="84" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>100</v>
       </c>
@@ -16012,7 +16025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -16134,7 +16147,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="86" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -16184,7 +16197,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="87" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -16225,7 +16238,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="88" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>181</v>
       </c>
@@ -16287,7 +16300,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="89" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -16355,7 +16368,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="90" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>181</v>
       </c>
@@ -16411,7 +16424,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="91" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>181</v>
       </c>
@@ -16461,7 +16474,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="92" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -16505,7 +16518,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="93" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>181</v>
       </c>
@@ -16555,7 +16568,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="94" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>181</v>
       </c>
@@ -16611,7 +16624,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="95" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>181</v>
       </c>
@@ -16667,7 +16680,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="96" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>181</v>
       </c>
@@ -16717,7 +16730,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="97" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>181</v>
       </c>
@@ -16779,7 +16792,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="98" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -16823,7 +16836,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="99" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>181</v>
       </c>
@@ -16879,7 +16892,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="100" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>181</v>
       </c>
@@ -16929,7 +16942,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="101" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>181</v>
       </c>
@@ -16979,7 +16992,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="102" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>181</v>
       </c>
@@ -17029,7 +17042,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="103" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>181</v>
       </c>
@@ -17097,7 +17110,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="104" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>181</v>
       </c>
@@ -17141,7 +17154,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="105" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>181</v>
       </c>
@@ -17203,7 +17216,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="106" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>181</v>
       </c>
@@ -17253,7 +17266,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="107" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>181</v>
       </c>
@@ -17309,7 +17322,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="108" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>181</v>
       </c>
@@ -17365,7 +17378,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="109" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>181</v>
       </c>
@@ -17415,7 +17428,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="110" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>181</v>
       </c>
@@ -17459,7 +17472,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="111" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>181</v>
       </c>
@@ -17518,7 +17531,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="112" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>181</v>
       </c>
@@ -17568,7 +17581,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="113" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>181</v>
       </c>
@@ -17594,7 +17607,7 @@
         <v>1</v>
       </c>
       <c r="N113" t="s">
-        <v>209</v>
+        <v>507</v>
       </c>
       <c r="O113" t="s">
         <v>208</v>
@@ -17642,7 +17655,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="114" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>181</v>
       </c>
@@ -17695,7 +17708,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="115" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>181</v>
       </c>
@@ -17739,7 +17752,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>181</v>
       </c>
@@ -17792,7 +17805,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="117" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>181</v>
       </c>
@@ -17845,7 +17858,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="118" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>181</v>
       </c>
@@ -17904,7 +17917,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="119" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>181</v>
       </c>
@@ -17954,7 +17967,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="120" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>181</v>
       </c>
@@ -17980,7 +17993,7 @@
         <v>1</v>
       </c>
       <c r="N120" t="s">
-        <v>209</v>
+        <v>507</v>
       </c>
       <c r="O120" t="s">
         <v>208</v>
@@ -18028,7 +18041,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="121" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>181</v>
       </c>
@@ -18081,7 +18094,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="122" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>181</v>
       </c>
@@ -18125,7 +18138,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="123" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>181</v>
       </c>
@@ -18178,7 +18191,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="124" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>181</v>
       </c>
@@ -18231,7 +18244,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="125" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>181</v>
       </c>
@@ -18296,7 +18309,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="126" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>181</v>
       </c>
@@ -18346,7 +18359,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="127" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>181</v>
       </c>
@@ -18420,7 +18433,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="128" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>181</v>
       </c>
@@ -18473,7 +18486,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="129" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>181</v>
       </c>
@@ -18517,7 +18530,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="130" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>181</v>
       </c>
@@ -18570,7 +18583,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="131" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>181</v>
       </c>
@@ -18635,7 +18648,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="132" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>181</v>
       </c>
@@ -18685,7 +18698,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="133" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>181</v>
       </c>
@@ -18759,7 +18772,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="134" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>181</v>
       </c>
@@ -18812,7 +18825,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="135" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>181</v>
       </c>
@@ -18856,7 +18869,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="136" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>181</v>
       </c>
@@ -18909,7 +18922,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="137" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>181</v>
       </c>
@@ -18974,7 +18987,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="138" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>181</v>
       </c>
@@ -19024,7 +19037,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="139" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>181</v>
       </c>
@@ -19098,7 +19111,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="140" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>181</v>
       </c>
@@ -19151,7 +19164,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="141" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>181</v>
       </c>
@@ -19195,7 +19208,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="142" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>181</v>
       </c>
@@ -19248,7 +19261,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="143" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>181</v>
       </c>
@@ -19310,7 +19323,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="144" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>181</v>
       </c>
@@ -19360,7 +19373,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="145" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>181</v>
       </c>
@@ -19428,7 +19441,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="146" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>181</v>
       </c>
@@ -19484,7 +19497,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="147" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>181</v>
       </c>
@@ -19528,7 +19541,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="148" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>181</v>
       </c>
@@ -19572,7 +19585,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="149" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>181</v>
       </c>
@@ -19640,7 +19653,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="150" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>181</v>
       </c>
@@ -19702,7 +19715,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="151" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>181</v>
       </c>
@@ -19764,7 +19777,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="152" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>181</v>
       </c>
@@ -19814,7 +19827,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="153" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>181</v>
       </c>
@@ -19858,7 +19871,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="154" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>181</v>
       </c>
@@ -19935,7 +19948,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="155" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>181</v>
       </c>
@@ -20006,7 +20019,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="156" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>181</v>
       </c>
@@ -20059,7 +20072,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="157" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>181</v>
       </c>
@@ -20112,7 +20125,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="158" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>181</v>
       </c>
@@ -20156,7 +20169,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="159" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>181</v>
       </c>
@@ -20230,7 +20243,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="160" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>181</v>
       </c>
@@ -20304,7 +20317,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="161" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>181</v>
       </c>
@@ -20357,7 +20370,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="162" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>181</v>
       </c>
@@ -20410,7 +20423,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="163" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>181</v>
       </c>
@@ -20454,7 +20467,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="164" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>181</v>
       </c>
@@ -20528,7 +20541,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="165" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>181</v>
       </c>
@@ -20602,7 +20615,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="166" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>181</v>
       </c>
@@ -20655,7 +20668,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="167" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>181</v>
       </c>
@@ -20708,7 +20721,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="168" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>181</v>
       </c>
@@ -20752,7 +20765,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="169" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>181</v>
       </c>
@@ -20826,7 +20839,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="170" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>181</v>
       </c>
@@ -20900,7 +20913,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="171" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>181</v>
       </c>
@@ -20953,7 +20966,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="172" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>181</v>
       </c>
@@ -21006,7 +21019,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="173" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>181</v>
       </c>
@@ -21050,7 +21063,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="174" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -21124,7 +21137,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="175" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -21180,7 +21193,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="176" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>181</v>
       </c>
@@ -21236,7 +21249,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="177" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>181</v>
       </c>
@@ -21289,7 +21302,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="178" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>181</v>
       </c>
@@ -21342,7 +21355,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="179" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>181</v>
       </c>
@@ -21386,7 +21399,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="180" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -21442,7 +21455,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="181" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>181</v>
       </c>
@@ -21495,7 +21508,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="182" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -21572,7 +21585,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="183" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -21625,7 +21638,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="184" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -21678,7 +21691,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="185" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>181</v>
       </c>
@@ -21722,7 +21735,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="186" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>181</v>
       </c>
@@ -21784,7 +21797,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="187" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>181</v>
       </c>
@@ -21846,7 +21859,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="188" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>181</v>
       </c>
@@ -21908,7 +21921,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="189" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>181</v>
       </c>
@@ -21952,7 +21965,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="190" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>181</v>
       </c>
@@ -22005,7 +22018,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="191" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>181</v>
       </c>
@@ -22058,7 +22071,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="192" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>181</v>
       </c>
@@ -22120,7 +22133,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="193" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>181</v>
       </c>
@@ -22170,7 +22183,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="194" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>181</v>
       </c>
@@ -22220,7 +22233,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="195" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>181</v>
       </c>
@@ -22282,7 +22295,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="196" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>181</v>
       </c>
@@ -22326,7 +22339,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="197" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>181</v>
       </c>
@@ -22379,7 +22392,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="198" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>181</v>
       </c>
@@ -22432,7 +22445,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="199" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>181</v>
       </c>
@@ -22494,7 +22507,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="200" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>181</v>
       </c>
@@ -22556,7 +22569,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="201" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>181</v>
       </c>
@@ -22612,7 +22625,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="202" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>181</v>
       </c>
@@ -22656,7 +22669,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="203" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>181</v>
       </c>
@@ -22700,7 +22713,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="204" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>181</v>
       </c>
@@ -22753,7 +22766,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="205" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>181</v>
       </c>
@@ -22806,7 +22819,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="206" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>181</v>
       </c>
@@ -22868,7 +22881,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="207" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>181</v>
       </c>
@@ -22924,7 +22937,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="208" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>181</v>
       </c>
@@ -22974,7 +22987,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="209" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>181</v>
       </c>
@@ -23018,7 +23031,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="210" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>181</v>
       </c>
@@ -23071,7 +23084,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="211" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>181</v>
       </c>
@@ -23124,7 +23137,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="212" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>181</v>
       </c>
@@ -23177,7 +23190,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="213" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>181</v>
       </c>
@@ -23239,7 +23252,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="214" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>181</v>
       </c>
@@ -23295,7 +23308,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="215" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>181</v>
       </c>
@@ -23345,7 +23358,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="216" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>181</v>
       </c>
@@ -23389,7 +23402,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="217" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>181</v>
       </c>
@@ -23442,7 +23455,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="218" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>181</v>
       </c>
@@ -23495,7 +23508,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="219" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>181</v>
       </c>
@@ -23548,7 +23561,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="220" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>181</v>
       </c>
@@ -23634,7 +23647,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="221" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>181</v>
       </c>
@@ -23696,7 +23709,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="222" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>181</v>
       </c>
@@ -23749,7 +23762,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="223" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>181</v>
       </c>
@@ -23802,7 +23815,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="224" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>181</v>
       </c>
@@ -23846,7 +23859,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="225" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>181</v>
       </c>
@@ -23932,7 +23945,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="226" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>181</v>
       </c>
@@ -23994,7 +24007,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="227" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>181</v>
       </c>
@@ -24047,7 +24060,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="228" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>181</v>
       </c>
@@ -24100,7 +24113,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="229" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>181</v>
       </c>
@@ -24144,7 +24157,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="230" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>289</v>
       </c>
@@ -24200,7 +24213,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="231" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>289</v>
       </c>
@@ -24250,7 +24263,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="232" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>289</v>
       </c>
@@ -24309,7 +24322,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="233" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>289</v>
       </c>
@@ -24362,7 +24375,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="234" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>289</v>
       </c>
@@ -24421,7 +24434,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="235" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>289</v>
       </c>
@@ -24477,7 +24490,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="236" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>289</v>
       </c>
@@ -24533,7 +24546,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="237" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>289</v>
       </c>
@@ -24583,7 +24596,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="238" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>289</v>
       </c>
@@ -24633,7 +24646,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="239" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>289</v>
       </c>
@@ -24698,7 +24711,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="240" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>289</v>
       </c>
@@ -24763,7 +24776,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="241" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>289</v>
       </c>
@@ -24816,7 +24829,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="242" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>289</v>
       </c>
@@ -24872,7 +24885,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="243" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>289</v>
       </c>
@@ -24922,7 +24935,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="244" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>289</v>
       </c>
@@ -24972,7 +24985,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="245" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>289</v>
       </c>
@@ -25022,7 +25035,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="246" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>289</v>
       </c>
@@ -25087,7 +25100,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="247" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>289</v>
       </c>
@@ -25146,7 +25159,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="248" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>289</v>
       </c>
@@ -25193,7 +25206,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="249" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>289</v>
       </c>
@@ -25249,7 +25262,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="250" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>289</v>
       </c>
@@ -25296,7 +25309,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="251" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>289</v>
       </c>
@@ -25361,7 +25374,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="252" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>289</v>
       </c>
@@ -25444,7 +25457,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="253" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>289</v>
       </c>
@@ -25494,7 +25507,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="254" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>289</v>
       </c>
@@ -25541,7 +25554,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="255" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>289</v>
       </c>
@@ -25591,7 +25604,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="256" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>289</v>
       </c>
@@ -25641,7 +25654,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="257" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>289</v>
       </c>
@@ -25688,7 +25701,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="258" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>289</v>
       </c>
@@ -25735,7 +25748,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="259" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>289</v>
       </c>
@@ -25776,7 +25789,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="260" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>289</v>
       </c>
@@ -25832,7 +25845,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="261" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>289</v>
       </c>
@@ -25882,7 +25895,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="262" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>289</v>
       </c>
@@ -25932,7 +25945,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="263" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>289</v>
       </c>
@@ -25979,7 +25992,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="264" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>289</v>
       </c>
@@ -26029,7 +26042,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="265" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>289</v>
       </c>
@@ -26079,7 +26092,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="266" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>289</v>
       </c>
@@ -26126,7 +26139,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="267" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>289</v>
       </c>
@@ -26173,7 +26186,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="268" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>289</v>
       </c>
@@ -26214,7 +26227,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="269" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>289</v>
       </c>
@@ -26264,7 +26277,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="270" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>289</v>
       </c>
@@ -26314,7 +26327,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="271" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>289</v>
       </c>
@@ -26370,7 +26383,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="272" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>289</v>
       </c>
@@ -26432,7 +26445,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="273" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>289</v>
       </c>
@@ -26494,7 +26507,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="274" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>289</v>
       </c>
@@ -26553,7 +26566,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="275" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>289</v>
       </c>
@@ -26609,7 +26622,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="276" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>289</v>
       </c>
@@ -26659,7 +26672,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="277" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>289</v>
       </c>
@@ -26706,7 +26719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>289</v>
       </c>
@@ -26753,7 +26766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>289</v>
       </c>
@@ -26800,7 +26813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>289</v>
       </c>
@@ -26847,7 +26860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>289</v>
       </c>
@@ -26888,7 +26901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>289</v>
       </c>
@@ -26944,7 +26957,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="283" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>289</v>
       </c>
@@ -26994,7 +27007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>289</v>
       </c>
@@ -27044,7 +27057,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="285" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>289</v>
       </c>
@@ -27094,7 +27107,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="286" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>355</v>
       </c>
@@ -27204,7 +27217,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="287" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>355</v>
       </c>
@@ -27254,7 +27267,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="288" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>355</v>
       </c>
@@ -27304,7 +27317,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="289" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>355</v>
       </c>
@@ -27390,7 +27403,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="290" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>355</v>
       </c>
@@ -27437,7 +27450,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="291" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>355</v>
       </c>
@@ -27508,7 +27521,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="292" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>355</v>
       </c>
@@ -27564,7 +27577,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="293" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>355</v>
       </c>
@@ -27614,7 +27627,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="294" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>355</v>
       </c>
@@ -27736,7 +27749,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="295" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>355</v>
       </c>
@@ -27786,7 +27799,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="296" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>355</v>
       </c>
@@ -27842,7 +27855,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="297" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>355</v>
       </c>
@@ -27970,7 +27983,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="298" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>355</v>
       </c>
@@ -28020,7 +28033,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="299" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>355</v>
       </c>
@@ -28079,7 +28092,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="300" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>355</v>
       </c>
@@ -28132,7 +28145,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="301" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>355</v>
       </c>
@@ -28191,7 +28204,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="302" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>355</v>
       </c>
@@ -28241,7 +28254,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="303" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>355</v>
       </c>
@@ -28282,7 +28295,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="304" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>355</v>
       </c>
@@ -28332,7 +28345,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="305" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>355</v>
       </c>
@@ -28382,7 +28395,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="306" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>355</v>
       </c>
@@ -28432,7 +28445,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="307" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>355</v>
       </c>
@@ -28554,7 +28567,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="308" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>355</v>
       </c>
@@ -28604,7 +28617,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="309" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>355</v>
       </c>
@@ -28660,7 +28673,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="310" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>355</v>
       </c>
@@ -28707,7 +28720,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="311" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>355</v>
       </c>
@@ -28796,7 +28809,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="312" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>355</v>
       </c>
@@ -28852,7 +28865,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="313" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>355</v>
       </c>
@@ -28902,7 +28915,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="314" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>355</v>
       </c>
@@ -28952,7 +28965,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="315" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>355</v>
       </c>
@@ -29002,7 +29015,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="316" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>355</v>
       </c>
@@ -29055,7 +29068,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="317" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>355</v>
       </c>
@@ -29159,7 +29172,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="318" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>355</v>
       </c>
@@ -29209,7 +29222,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="319" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>355</v>
       </c>
@@ -29259,7 +29272,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="320" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>355</v>
       </c>
@@ -29309,7 +29322,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="321" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>355</v>
       </c>
@@ -29362,7 +29375,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="322" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>355</v>
       </c>
@@ -29472,7 +29485,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="323" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>355</v>
       </c>
@@ -29528,7 +29541,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="324" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>355</v>
       </c>
@@ -29578,7 +29591,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="325" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>405</v>
       </c>
@@ -29637,7 +29650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>405</v>
       </c>
@@ -29684,7 +29697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>405</v>
       </c>
@@ -29740,7 +29753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>405</v>
       </c>
@@ -29793,7 +29806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>405</v>
       </c>
@@ -29843,7 +29856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>405</v>
       </c>
@@ -29887,7 +29900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>405</v>
       </c>
@@ -29937,7 +29950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>405</v>
       </c>
@@ -29987,7 +30000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>405</v>
       </c>
@@ -30052,7 +30065,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="334" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>405</v>
       </c>
@@ -30111,7 +30124,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="335" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>405</v>
       </c>
@@ -30158,7 +30171,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="336" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>405</v>
       </c>
@@ -30208,7 +30221,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="337" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>405</v>
       </c>
@@ -30249,7 +30262,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="338" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>405</v>
       </c>
@@ -30293,7 +30306,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="339" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>405</v>
       </c>
@@ -30367,7 +30380,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="340" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>405</v>
       </c>
@@ -30432,7 +30445,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="341" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>405</v>
       </c>
@@ -30497,7 +30510,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="342" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>405</v>
       </c>
@@ -30541,7 +30554,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="343" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>405</v>
       </c>
@@ -30600,7 +30613,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="344" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>405</v>
       </c>
@@ -30665,7 +30678,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="345" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>405</v>
       </c>
@@ -30730,7 +30743,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="346" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>405</v>
       </c>
@@ -30771,7 +30784,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="347" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>405</v>
       </c>
@@ -30836,7 +30849,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="348" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>405</v>
       </c>
@@ -30895,7 +30908,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="349" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>405</v>
       </c>
@@ -30954,7 +30967,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="350" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>405</v>
       </c>
@@ -30995,7 +31008,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="351" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>405</v>
       </c>
@@ -31036,7 +31049,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="352" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>405</v>
       </c>
@@ -31095,7 +31108,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="353" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>405</v>
       </c>
@@ -31142,7 +31155,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="354" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>405</v>
       </c>
@@ -31189,7 +31202,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="355" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>405</v>
       </c>
@@ -31254,7 +31267,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="356" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>405</v>
       </c>
@@ -31295,7 +31308,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="357" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>405</v>
       </c>
@@ -31336,7 +31349,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="358" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>405</v>
       </c>
@@ -31401,7 +31414,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="359" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>405</v>
       </c>
@@ -31460,7 +31473,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="360" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>405</v>
       </c>
@@ -31528,7 +31541,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="361" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>405</v>
       </c>
@@ -31572,7 +31585,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="362" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>405</v>
       </c>
@@ -31613,7 +31626,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="363" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>405</v>
       </c>
@@ -31672,7 +31685,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="364" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>405</v>
       </c>
@@ -31737,7 +31750,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="365" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>405</v>
       </c>
@@ -31796,7 +31809,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="366" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>405</v>
       </c>
@@ -31837,7 +31850,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="367" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>405</v>
       </c>
@@ -31878,7 +31891,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="368" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>405</v>
       </c>
@@ -31946,7 +31959,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="369" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>405</v>
       </c>
@@ -32005,7 +32018,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="370" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>405</v>
       </c>
@@ -32070,7 +32083,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="371" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>405</v>
       </c>
@@ -32111,7 +32124,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="372" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>405</v>
       </c>
@@ -32155,7 +32168,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="373" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>405</v>
       </c>
@@ -32220,7 +32233,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="374" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>405</v>
       </c>
@@ -32279,7 +32292,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="375" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>405</v>
       </c>
@@ -32341,7 +32354,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="376" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>405</v>
       </c>
@@ -32382,7 +32395,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="377" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>405</v>
       </c>
@@ -32423,7 +32436,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="378" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>405</v>
       </c>
@@ -32467,7 +32480,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="379" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:105" x14ac:dyDescent="0.3">
       <c r="R379">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[6-7L])</f>
         <v>32</v>
@@ -32846,7 +32859,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R379:DA379">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32874,15 +32887,15 @@
       <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>465</v>
       </c>
@@ -32890,7 +32903,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>157</v>
       </c>
@@ -32898,7 +32911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>198</v>
       </c>
@@ -32906,7 +32919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>310</v>
       </c>
@@ -32914,7 +32927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>186</v>
       </c>
@@ -32922,7 +32935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>422</v>
       </c>
@@ -32930,7 +32943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>379</v>
       </c>
@@ -32938,7 +32951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>410</v>
       </c>
@@ -32946,7 +32959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>106</v>
       </c>
@@ -32954,7 +32967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>448</v>
       </c>
@@ -32962,7 +32975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>126</v>
       </c>
@@ -32970,7 +32983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>466</v>
       </c>
@@ -32978,7 +32991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>235</v>
       </c>
@@ -32986,7 +32999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>467</v>
       </c>
@@ -32994,7 +33007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -33002,7 +33015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>468</v>
       </c>
@@ -33010,7 +33023,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>309</v>
       </c>
@@ -33018,7 +33031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>469</v>
       </c>
@@ -33026,7 +33039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>424</v>
       </c>
@@ -33034,7 +33047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>426</v>
       </c>
@@ -33042,7 +33055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>195</v>
       </c>
@@ -33050,7 +33063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>117</v>
       </c>
@@ -33058,7 +33071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>217</v>
       </c>
@@ -33066,7 +33079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>408</v>
       </c>
@@ -33074,7 +33087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>470</v>
       </c>
@@ -33082,7 +33095,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>471</v>
       </c>
@@ -33090,7 +33103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>472</v>
       </c>
@@ -33098,7 +33111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>163</v>
       </c>
@@ -33112,7 +33125,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>371</v>
       </c>
@@ -33126,7 +33139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>142</v>
       </c>
@@ -33140,7 +33153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>139</v>
       </c>
@@ -33154,7 +33167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>165</v>
       </c>
@@ -33168,7 +33181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>375</v>
       </c>
@@ -33182,7 +33195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>128</v>
       </c>
@@ -33196,7 +33209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>358</v>
       </c>
@@ -33210,7 +33223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>226</v>
       </c>
@@ -33224,7 +33237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>223</v>
       </c>
@@ -33238,7 +33251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>114</v>
       </c>
@@ -33252,7 +33265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>403</v>
       </c>
@@ -33266,7 +33279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>250</v>
       </c>
@@ -33280,7 +33293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>366</v>
       </c>
@@ -33294,7 +33307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>194</v>
       </c>
@@ -33308,7 +33321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>159</v>
       </c>
@@ -33322,7 +33335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>150</v>
       </c>
@@ -33336,7 +33349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>151</v>
       </c>
@@ -33350,7 +33363,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>124</v>
       </c>
@@ -33358,7 +33371,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>180</v>
       </c>
@@ -33366,7 +33379,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>272</v>
       </c>
@@ -33374,7 +33387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>335</v>
       </c>
@@ -33382,7 +33395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>473</v>
       </c>
@@ -33390,7 +33403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>444</v>
       </c>
@@ -33398,7 +33411,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>120</v>
       </c>
@@ -33406,7 +33419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>173</v>
       </c>
@@ -33414,7 +33427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>389</v>
       </c>
@@ -33422,7 +33435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>221</v>
       </c>
@@ -33430,7 +33443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>292</v>
       </c>
@@ -33438,7 +33451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>111</v>
       </c>
@@ -33446,7 +33459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>189</v>
       </c>
@@ -33454,7 +33467,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>398</v>
       </c>
@@ -33462,7 +33475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>474</v>
       </c>
@@ -33470,7 +33483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>209</v>
       </c>
@@ -33478,7 +33491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>257</v>
       </c>
@@ -33486,7 +33499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>481</v>
       </c>
@@ -33494,7 +33507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>303</v>
       </c>
@@ -33502,7 +33515,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>480</v>
       </c>
@@ -33510,7 +33523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>479</v>
       </c>
@@ -33518,7 +33531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>152</v>
       </c>
@@ -33526,7 +33539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>301</v>
       </c>
@@ -33534,7 +33547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>133</v>
       </c>
@@ -33542,7 +33555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>103</v>
       </c>
@@ -33550,7 +33563,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>420</v>
       </c>
@@ -33558,7 +33571,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>364</v>
       </c>
@@ -33566,7 +33579,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>487</v>
       </c>
@@ -33574,7 +33587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>220</v>
       </c>
@@ -33582,7 +33595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>475</v>
       </c>
@@ -33590,7 +33603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>136</v>
       </c>
@@ -33598,7 +33611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>197</v>
       </c>
@@ -33606,7 +33619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
@@ -33614,7 +33627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>131</v>
       </c>
@@ -33622,7 +33635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>476</v>
       </c>

</xml_diff>